<commit_message>
functions for date and time is added
</commit_message>
<xml_diff>
--- a/ProductionDataLog.xlsx
+++ b/ProductionDataLog.xlsx
@@ -355,7 +355,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -405,7 +405,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -422,6 +422,16 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B1:B233" displayName="Table1" name="Table1" id="1" totalsRowShown="0">
+  <autoFilter ref="B1:B233"/>
+  <tableColumns count="1">
+    <tableColumn name="Date" id="1" totalsRowLabel="Total"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showColumnStripes="0" showRowStripes="1" showLastColumn="0" showFirstColumn="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3356,7 +3366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="19.5">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -3391,7 +3401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="19.5">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -3426,7 +3436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="19.5">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -3461,7 +3471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="19.5">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -3496,7 +3506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="19.5">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -3531,7 +3541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="19.5">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -3566,7 +3576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="19.5">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -3601,7 +3611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="19.5">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -3636,7 +3646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="19.5">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -3671,7 +3681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="19.5">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -3706,7 +3716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="19.5">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -3741,7 +3751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="19.5">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -3776,7 +3786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="19.5">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -3811,7 +3821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="19.5">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -3846,7 +3856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="19.5">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -3881,7 +3891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="19.5">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -3916,7 +3926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="19.5">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -3951,7 +3961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="19.5">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -3986,7 +3996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="19.5">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -4021,7 +4031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="19.5">
       <c r="A95" s="3">
         <v>94</v>
       </c>
@@ -4056,7 +4066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="19.5">
       <c r="A96" s="3">
         <v>95</v>
       </c>
@@ -4091,7 +4101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="19.5">
       <c r="A97" s="3">
         <v>96</v>
       </c>
@@ -4126,7 +4136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="19.5">
       <c r="A98" s="3">
         <v>97</v>
       </c>
@@ -4161,7 +4171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="19.5">
       <c r="A99" s="3">
         <v>98</v>
       </c>
@@ -8888,5 +8898,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>